<commit_message>
Implement 'Verify Excel Specification' feature.
</commit_message>
<xml_diff>
--- a/fitnesse-connect-connect/src/test/fitnesse/files/sample/SampleTwo.xlsx
+++ b/fitnesse-connect-connect/src/test/fitnesse/files/sample/SampleTwo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FitNesseConnect\fitnesse-connect-connect\src\test\fitnesse\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\FitNesseConnect\fitnesse-connect-connect\src\test\fitnesse\files\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Column A</t>
   </si>
@@ -43,6 +43,39 @@
   </si>
   <si>
     <t>3_B</t>
+  </si>
+  <si>
+    <t>this is a text</t>
+  </si>
+  <si>
+    <t>this is another text</t>
+  </si>
+  <si>
+    <t>2016.12.09</t>
+  </si>
+  <si>
+    <t>2016.12.31</t>
+  </si>
+  <si>
+    <t>has value</t>
+  </si>
+  <si>
+    <t>String Column</t>
+  </si>
+  <si>
+    <t>Integer Column</t>
+  </si>
+  <si>
+    <t>Date Column</t>
+  </si>
+  <si>
+    <t>Optional Column</t>
+  </si>
+  <si>
+    <t>Optional Value Column</t>
+  </si>
+  <si>
+    <t>has another value</t>
   </si>
 </sst>
 </file>
@@ -360,36 +393,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>